<commit_message>
v1.6 Cambio de la interfaz de archivos
a una pestaña de la misma interfaz PS3 cambios en la creación de PDF orden del código de creación de directorios
</commit_message>
<xml_diff>
--- a/Destalle de Juegos.xlsx
+++ b/Destalle de Juegos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\march\Google Drive\Aplicaciones\JAVA\Juegos Listo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\march\Documents\GitHub\Juegos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05256B32-4532-402E-AD7C-5893ADAB2E72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC74DE4-CDB4-4A1A-A0AC-87371ACAFDB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="4080" windowWidth="15165" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13350" yWindow="3015" windowWidth="15165" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PSX" sheetId="1" r:id="rId1"/>
@@ -22162,8 +22162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="A154" sqref="A154:I154"/>
+    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
+      <selection activeCell="A155" sqref="A155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -22204,7 +22204,7 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="2" t="s">
         <v>184</v>
       </c>
       <c r="B2" s="12" t="s">
@@ -22305,7 +22305,7 @@
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="2" t="s">
         <v>1231</v>
       </c>
       <c r="B6" s="12" t="s">
@@ -22777,7 +22777,7 @@
       </c>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="2" t="s">
         <v>1259</v>
       </c>
       <c r="B26" s="12" t="s">
@@ -22852,7 +22852,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" s="32" customFormat="1">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="25" t="s">
         <v>1750</v>
       </c>
       <c r="B29" s="14" t="s">
@@ -24709,7 +24709,7 @@
       </c>
     </row>
     <row r="110" spans="1:9">
-      <c r="A110" s="12" t="s">
+      <c r="A110" s="2" t="s">
         <v>1748</v>
       </c>
       <c r="B110" s="12" t="s">
@@ -25518,7 +25518,7 @@
       </c>
     </row>
     <row r="145" spans="1:9">
-      <c r="A145" s="12" t="s">
+      <c r="A145" s="2" t="s">
         <v>2028</v>
       </c>
       <c r="B145" s="12" t="s">
@@ -25547,7 +25547,7 @@
       </c>
     </row>
     <row r="146" spans="1:9">
-      <c r="A146" s="12" t="s">
+      <c r="A146" s="2" t="s">
         <v>2030</v>
       </c>
       <c r="B146" s="12" t="s">
@@ -25576,7 +25576,7 @@
       </c>
     </row>
     <row r="147" spans="1:9">
-      <c r="A147" s="12" t="s">
+      <c r="A147" s="2" t="s">
         <v>2036</v>
       </c>
       <c r="B147" s="12" t="s">
@@ -25605,7 +25605,7 @@
       </c>
     </row>
     <row r="148" spans="1:9">
-      <c r="A148" s="12" t="s">
+      <c r="A148" s="2" t="s">
         <v>2038</v>
       </c>
       <c r="B148" s="12" t="s">
@@ -25634,7 +25634,7 @@
       </c>
     </row>
     <row r="149" spans="1:9">
-      <c r="A149" s="12" t="s">
+      <c r="A149" s="2" t="s">
         <v>2040</v>
       </c>
       <c r="B149" s="12" t="s">
@@ -25690,7 +25690,7 @@
       </c>
     </row>
     <row r="151" spans="1:9">
-      <c r="A151" s="12" t="s">
+      <c r="A151" s="2" t="s">
         <v>2043</v>
       </c>
       <c r="B151" s="12" t="s">
@@ -25719,7 +25719,7 @@
       </c>
     </row>
     <row r="152" spans="1:9">
-      <c r="A152" s="12" t="s">
+      <c r="A152" s="2" t="s">
         <v>2050</v>
       </c>
       <c r="B152" s="12" t="s">
@@ -25748,7 +25748,7 @@
       </c>
     </row>
     <row r="153" spans="1:9">
-      <c r="A153" s="12" t="s">
+      <c r="A153" s="2" t="s">
         <v>2051</v>
       </c>
       <c r="B153" s="12" t="s">
@@ -25777,7 +25777,7 @@
       </c>
     </row>
     <row r="154" spans="1:9">
-      <c r="A154" s="12" t="s">
+      <c r="A154" s="2" t="s">
         <v>2052</v>
       </c>
       <c r="B154" s="12" t="s">
@@ -25806,7 +25806,7 @@
       </c>
     </row>
     <row r="155" spans="1:9">
-      <c r="A155" s="12" t="s">
+      <c r="A155" s="2" t="s">
         <v>2058</v>
       </c>
       <c r="B155" s="12" t="s">

</xml_diff>

<commit_message>
v1.8.3 Integracion de los datos
Se agrego datos al Excel para Trabajar la BD
</commit_message>
<xml_diff>
--- a/Destalle de Juegos.xlsx
+++ b/Destalle de Juegos.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\march\Documents\GitHub\Juegos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Juegos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC74DE4-CDB4-4A1A-A0AC-87371ACAFDB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1FB7BD-0D1C-41D0-AF53-AE5D95E11138}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13350" yWindow="3015" windowWidth="15165" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13965" yWindow="3360" windowWidth="16620" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PSX" sheetId="1" r:id="rId1"/>
     <sheet name="PS2" sheetId="2" r:id="rId2"/>
     <sheet name="PSP" sheetId="4" r:id="rId3"/>
     <sheet name="PS3" sheetId="3" r:id="rId4"/>
-    <sheet name="PC" sheetId="5" r:id="rId5"/>
-    <sheet name="Help" sheetId="6" r:id="rId6"/>
+    <sheet name="PS4" sheetId="7" r:id="rId5"/>
+    <sheet name="PC" sheetId="5" r:id="rId6"/>
+    <sheet name="Help" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'PS2'!$A$1:$A$291</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5376" uniqueCount="2064">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5405" uniqueCount="2071">
   <si>
     <t>ID</t>
   </si>
@@ -6239,6 +6240,27 @@
   </si>
   <si>
     <t>Revisar Vercion</t>
+  </si>
+  <si>
+    <t>CUSA04729</t>
+  </si>
+  <si>
+    <t>Cartoon Network Battle Crashers</t>
+  </si>
+  <si>
+    <t>PKG</t>
+  </si>
+  <si>
+    <t>CUSA07402</t>
+  </si>
+  <si>
+    <t>Crash.Bandicoot.N.Sane.Trilogy</t>
+  </si>
+  <si>
+    <t>CUSA13795</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crash Team Racing Nitro Fueled </t>
   </si>
 </sst>
 </file>
@@ -22162,8 +22184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="A155" sqref="A155"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -26307,6 +26329,134 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BFD6704-31D9-442F-B705-7B157B6AB9D0}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2066</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>2031</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>2064</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2065</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1406</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>133</v>
+      </c>
+      <c r="G2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2057</v>
+      </c>
+      <c r="I2" t="s">
+        <v>2057</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>2067</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2068</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>675</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>21.2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" t="s">
+        <v>2034</v>
+      </c>
+      <c r="I3" t="s">
+        <v>2057</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>2069</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2070</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>675</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>16.3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" t="s">
+        <v>2034</v>
+      </c>
+      <c r="I4" t="s">
+        <v>2034</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L170"/>
   <sheetViews>
@@ -31595,7 +31745,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L18"/>
   <sheetViews>

</xml_diff>

<commit_message>
v1.10 Implementación de versiones de update a la interfaz de PS4
registra las versiones de las actualizaciones de los Juegos registrados
</commit_message>
<xml_diff>
--- a/Destalle de Juegos.xlsx
+++ b/Destalle de Juegos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Juegos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1FB7BD-0D1C-41D0-AF53-AE5D95E11138}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AE270D-F7F7-44EA-882A-0D23FE96A0F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13965" yWindow="3360" windowWidth="16620" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7635" yWindow="1965" windowWidth="16620" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PSX" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5405" uniqueCount="2071">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5406" uniqueCount="2072">
   <si>
     <t>ID</t>
   </si>
@@ -6261,6 +6261,9 @@
   </si>
   <si>
     <t xml:space="preserve">Crash Team Racing Nitro Fueled </t>
+  </si>
+  <si>
+    <t>v PATCH</t>
   </si>
 </sst>
 </file>
@@ -6440,7 +6443,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -6493,6 +6496,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -26330,41 +26335,49 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BFD6704-31D9-442F-B705-7B157B6AB9D0}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="46"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>2066</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="G1" s="2"/>
+      <c r="H1" s="2" t="s">
         <v>2031</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="47" t="s">
+        <v>2071</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>2032</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>2064</v>
       </c>
@@ -26381,7 +26394,7 @@
         <v>4</v>
       </c>
       <c r="F2">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="G2" t="s">
         <v>91</v>
@@ -26389,11 +26402,14 @@
       <c r="H2" t="s">
         <v>2057</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="46">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
         <v>2057</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>2067</v>
       </c>
@@ -26410,7 +26426,7 @@
         <v>4</v>
       </c>
       <c r="F3">
-        <v>21.2</v>
+        <v>22.8</v>
       </c>
       <c r="G3" t="s">
         <v>76</v>
@@ -26418,11 +26434,14 @@
       <c r="H3" t="s">
         <v>2034</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="46">
+        <v>1.01</v>
+      </c>
+      <c r="J3" t="s">
         <v>2057</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>2069</v>
       </c>
@@ -26447,12 +26466,16 @@
       <c r="H4" t="s">
         <v>2034</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="46">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="J4" t="s">
         <v>2034</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>